<commit_message>
Update Data.go.th endpoint to csv
</commit_message>
<xml_diff>
--- a/New Wave Data🔥/xlsx/provinces-cases.xlsx
+++ b/New Wave Data🔥/xlsx/provinces-cases.xlsx
@@ -374,7 +374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A61"/>
+  <dimension ref="A1:A63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -387,27 +387,27 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>2210</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>930</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>927</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>500</v>
+        <v>509</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>328</v>
+        <v>387</v>
       </c>
     </row>
     <row r="7" spans="1:1">
@@ -417,47 +417,47 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>272</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -467,22 +467,22 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:1">
@@ -492,12 +492,12 @@
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:1">
@@ -507,17 +507,17 @@
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:1">
@@ -527,22 +527,22 @@
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:1">
@@ -562,12 +562,12 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:1">
@@ -577,7 +577,7 @@
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:1">
@@ -597,12 +597,12 @@
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:1">
@@ -632,7 +632,7 @@
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:1">
@@ -682,6 +682,16 @@
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test Extraction on Git ✨ 21 ม.ค. 64 เวลา 18:44
</commit_message>
<xml_diff>
--- a/New Wave Data🔥/xlsx/provinces-cases.xlsx
+++ b/New Wave Data🔥/xlsx/provinces-cases.xlsx
@@ -374,7 +374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A77"/>
+  <dimension ref="A1:A63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -387,381 +387,311 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>3607</v>
+        <v>3599</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>2136</v>
+        <v>773</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>1068</v>
+        <v>701</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>568</v>
+        <v>563</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>491</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>284</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>215</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>109</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <v>83</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <v>78</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <v>75</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <v>41</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77">
         <v>1</v>
       </c>
     </row>

</xml_diff>